<commit_message>
Obtain information from Title sheet
</commit_message>
<xml_diff>
--- a/Example_Spec_v1.0.xlsx
+++ b/Example_Spec_v1.0.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AD083DE-6831-4A0A-9570-EB9A1501F089}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F948446-5465-4040-86F0-2D46C4F6F2A8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Title" sheetId="3" r:id="rId1"/>
-    <sheet name="UDF Source" sheetId="5" r:id="rId2"/>
+    <sheet name="UDF" sheetId="5" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
@@ -805,7 +805,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated specs with sample rules
</commit_message>
<xml_diff>
--- a/Example_Spec_v1.0.xlsx
+++ b/Example_Spec_v1.0.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBD3DB26-2221-47AA-B24E-76DAB74BAFE7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F35DE598-9D69-4B90-B203-30A9E5F1C4E5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Title" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="122">
   <si>
     <t>Format</t>
   </si>
@@ -389,6 +389,50 @@
   </si>
   <si>
     <t>SE_Se01</t>
+  </si>
+  <si>
+    <t>1) 
+[]
+;;
+;; o------------------------------------------------------------------------------------------o
+;; |                   Map Documentation
+;; o------------------------------------------------------------------------------------------o
+;; |          GXS Client: MCHLN
+;; |             Program: MCHLNO2CoINVOICFFbs.mdl
+;; |           Direction: Outbound
+;; |            Standard: UDF
+;; |            Document: COMMON
+;; |             Version: COMMON
+;; |     Trading Partner: Daimler
+;; |  Corp/Customer Code: 
+;; |        Developed By: floresl
+;; |      Date Developed: Thu Aug 23 17:41:33 SGT 2012
+;; |    Last Modified By:
+;; |  Date Last Modified:
+;; o------------------------------------------------------------------------------------------o
+2) 
+[]
+  VAR-&gt;NULL = ""
+  VAR-&gt;TRIM_TYPE = "B"
+  VAR-&gt;SPACE = " "
+  VAR-&gt;DATA = "Data"
+  VAR-&gt;STOP = "Stop"
+  VAR-&gt;YES = "Yes"
+  VAR-&gt;NO = "No"
+3) 
+[]
+  VAR-&gt;Workbench = VAR-&gt;YES
+  VAR-&gt;Session = VAR-&gt;NULL
+  VAR-&gt;Session = VAR-&gt;OTSessionNo
+[VAR-&gt;Session != VAR-&gt;NULL]
+  VAR-&gt;Workbench = VAR-&gt;NO
+[VAR-&gt;Workbench == VAR-&gt;YES]
+  PERFORM("OTSessionInit")
+4) 
+[]
+  ;;; ECSC Standard Map PERFORM
+  PERFORM ("ECSCOutbSourceInit")
+  PERFORM ("OTAdminInit")</t>
   </si>
 </sst>
 </file>
@@ -482,7 +526,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -518,6 +562,9 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -804,7 +851,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8045FFDE-9538-4935-B0FE-47BFD07C873D}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -928,7 +975,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A63BC555-24CF-4E67-AB49-71FACE572BA7}">
   <dimension ref="A1:N49"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -945,7 +994,7 @@
     <col min="11" max="11" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="21.140625" customWidth="1"/>
     <col min="13" max="13" width="20.28515625" customWidth="1"/>
-    <col min="14" max="14" width="25.140625" customWidth="1"/>
+    <col min="14" max="14" width="40.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="26.25" x14ac:dyDescent="0.25">
@@ -992,7 +1041,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
@@ -1014,7 +1063,9 @@
       <c r="M2" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="N2" s="9"/>
+      <c r="N2" s="14" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="3" spans="1:14" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">

</xml_diff>

<commit_message>
Added additional field formats
</commit_message>
<xml_diff>
--- a/Example_Spec_v1.0.xlsx
+++ b/Example_Spec_v1.0.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F35DE598-9D69-4B90-B203-30A9E5F1C4E5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA8C8FE0-8896-4FC0-8AA3-B98E3045D265}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="125">
   <si>
     <t>Format</t>
   </si>
@@ -391,48 +391,16 @@
     <t>SE_Se01</t>
   </si>
   <si>
-    <t>1) 
-[]
-;;
-;; o------------------------------------------------------------------------------------------o
-;; |                   Map Documentation
-;; o------------------------------------------------------------------------------------------o
-;; |          GXS Client: MCHLN
-;; |             Program: MCHLNO2CoINVOICFFbs.mdl
-;; |           Direction: Outbound
-;; |            Standard: UDF
-;; |            Document: COMMON
-;; |             Version: COMMON
-;; |     Trading Partner: Daimler
-;; |  Corp/Customer Code: 
-;; |        Developed By: floresl
-;; |      Date Developed: Thu Aug 23 17:41:33 SGT 2012
-;; |    Last Modified By:
-;; |  Date Last Modified:
-;; o------------------------------------------------------------------------------------------o
-2) 
-[]
-  VAR-&gt;NULL = ""
-  VAR-&gt;TRIM_TYPE = "B"
-  VAR-&gt;SPACE = " "
-  VAR-&gt;DATA = "Data"
-  VAR-&gt;STOP = "Stop"
-  VAR-&gt;YES = "Yes"
-  VAR-&gt;NO = "No"
-3) 
-[]
-  VAR-&gt;Workbench = VAR-&gt;YES
-  VAR-&gt;Session = VAR-&gt;NULL
-  VAR-&gt;Session = VAR-&gt;OTSessionNo
-[VAR-&gt;Session != VAR-&gt;NULL]
-  VAR-&gt;Workbench = VAR-&gt;NO
-[VAR-&gt;Workbench == VAR-&gt;YES]
-  PERFORM("OTSessionInit")
-4) 
-[]
-  ;;; ECSC Standard Map PERFORM
-  PERFORM ("ECSCOutbSourceInit")
-  PERFORM ("OTAdminInit")</t>
+    <t>HDR_Date</t>
+  </si>
+  <si>
+    <t>DT</t>
+  </si>
+  <si>
+    <t>YYYYMMDD</t>
+  </si>
+  <si>
+    <t>NF</t>
   </si>
 </sst>
 </file>
@@ -852,7 +820,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -973,10 +941,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A63BC555-24CF-4E67-AB49-71FACE572BA7}">
-  <dimension ref="A1:N49"/>
+  <dimension ref="A1:N50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -986,7 +954,7 @@
     <col min="3" max="3" width="34.28515625" customWidth="1"/>
     <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.28515625" bestFit="1" customWidth="1"/>
@@ -1041,7 +1009,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
@@ -1063,9 +1031,7 @@
       <c r="M2" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="N2" s="14" t="s">
-        <v>121</v>
-      </c>
+      <c r="N2" s="14"/>
     </row>
     <row r="3" spans="1:14" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
@@ -1210,11 +1176,11 @@
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
       <c r="G8" s="11">
-        <f t="shared" ref="G8:G28" si="0">+H7+1</f>
+        <f t="shared" ref="G8:G29" si="0">+H7+1</f>
         <v>7</v>
       </c>
       <c r="H8" s="11">
-        <f t="shared" ref="H8:H28" si="1">+H7+I8</f>
+        <f t="shared" ref="H8:H29" si="1">+H7+I8</f>
         <v>15</v>
       </c>
       <c r="I8" s="11">
@@ -1228,7 +1194,7 @@
       <c r="M8" s="12"/>
       <c r="N8" s="11"/>
     </row>
-    <row r="9" spans="1:14" ht="39" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A9" s="11"/>
       <c r="B9" s="11" t="s">
         <v>65</v>
@@ -1264,7 +1230,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="39" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A10" s="11"/>
       <c r="B10" s="11" t="s">
         <v>68</v>
@@ -1388,7 +1354,7 @@
       <c r="M13" s="12"/>
       <c r="N13" s="11"/>
     </row>
-    <row r="14" spans="1:14" ht="39" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A14" s="11"/>
       <c r="B14" s="11" t="s">
         <v>75</v>
@@ -1424,7 +1390,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="39" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A15" s="11"/>
       <c r="B15" s="11" t="s">
         <v>78</v>
@@ -1463,24 +1429,26 @@
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="11"/>
       <c r="B16" s="11" t="s">
-        <v>81</v>
+        <v>121</v>
       </c>
       <c r="C16" s="11"/>
       <c r="D16" s="11" t="s">
-        <v>37</v>
+        <v>122</v>
       </c>
       <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
+      <c r="F16" s="11" t="s">
+        <v>123</v>
+      </c>
       <c r="G16" s="11">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="H16" s="11">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="I16" s="11">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J16" s="11" t="s">
         <v>36</v>
@@ -1490,12 +1458,12 @@
       </c>
       <c r="L16" s="12"/>
       <c r="M16" s="12"/>
-      <c r="N16" s="13"/>
+      <c r="N16" s="12"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="11"/>
       <c r="B17" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C17" s="11"/>
       <c r="D17" s="11" t="s">
@@ -1504,28 +1472,28 @@
       <c r="E17" s="11"/>
       <c r="F17" s="11"/>
       <c r="G17" s="11">
-        <f t="shared" si="0"/>
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="H17" s="11">
-        <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="I17" s="11">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="J17" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="K17" s="11"/>
+      <c r="K17" s="11" t="s">
+        <v>53</v>
+      </c>
       <c r="L17" s="12"/>
       <c r="M17" s="12"/>
-      <c r="N17" s="12"/>
+      <c r="N17" s="13"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="11"/>
       <c r="B18" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C18" s="11"/>
       <c r="D18" s="11" t="s">
@@ -1539,10 +1507,10 @@
       </c>
       <c r="H18" s="11">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="I18" s="11">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J18" s="11" t="s">
         <v>36</v>
@@ -1550,12 +1518,12 @@
       <c r="K18" s="11"/>
       <c r="L18" s="12"/>
       <c r="M18" s="12"/>
-      <c r="N18" s="11"/>
+      <c r="N18" s="12"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="11"/>
       <c r="B19" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C19" s="11"/>
       <c r="D19" s="11" t="s">
@@ -1565,14 +1533,14 @@
       <c r="F19" s="11"/>
       <c r="G19" s="11">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="H19" s="11">
         <f t="shared" si="1"/>
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="I19" s="11">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="J19" s="11" t="s">
         <v>36</v>
@@ -1585,7 +1553,7 @@
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="11"/>
       <c r="B20" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C20" s="11"/>
       <c r="D20" s="11" t="s">
@@ -1595,14 +1563,14 @@
       <c r="F20" s="11"/>
       <c r="G20" s="11">
         <f t="shared" si="0"/>
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="H20" s="11">
         <f t="shared" si="1"/>
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="I20" s="11">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="J20" s="11" t="s">
         <v>36</v>
@@ -1615,7 +1583,7 @@
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="11"/>
       <c r="B21" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C21" s="11"/>
       <c r="D21" s="11" t="s">
@@ -1625,14 +1593,14 @@
       <c r="F21" s="11"/>
       <c r="G21" s="11">
         <f t="shared" si="0"/>
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="H21" s="11">
         <f t="shared" si="1"/>
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="I21" s="11">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J21" s="11" t="s">
         <v>36</v>
@@ -1643,21 +1611,29 @@
       <c r="N21" s="11"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="B22" s="11"/>
+      <c r="A22" s="11"/>
+      <c r="B22" s="11" t="s">
+        <v>86</v>
+      </c>
       <c r="C22" s="11"/>
       <c r="D22" s="11" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E22" s="11"/>
       <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
+      <c r="G22" s="11">
+        <f t="shared" si="0"/>
+        <v>71</v>
+      </c>
+      <c r="H22" s="11">
+        <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
+      <c r="I22" s="11">
+        <v>5</v>
+      </c>
       <c r="J22" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="K22" s="11"/>
       <c r="L22" s="12"/>
@@ -1665,71 +1641,63 @@
       <c r="N22" s="11"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="11"/>
-      <c r="B23" s="11" t="s">
-        <v>88</v>
-      </c>
+      <c r="A23" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="B23" s="11"/>
       <c r="C23" s="11"/>
       <c r="D23" s="11" t="s">
-        <v>61</v>
+        <v>34</v>
       </c>
       <c r="E23" s="11"/>
       <c r="F23" s="11"/>
-      <c r="G23" s="11">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H23" s="11">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="I23" s="11">
-        <v>3</v>
-      </c>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
       <c r="J23" s="11" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="K23" s="11"/>
-      <c r="L23" s="12" t="s">
-        <v>89</v>
-      </c>
+      <c r="L23" s="12"/>
       <c r="M23" s="12"/>
       <c r="N23" s="11"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="11"/>
       <c r="B24" s="11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C24" s="11"/>
       <c r="D24" s="11" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="E24" s="11"/>
       <c r="F24" s="11"/>
       <c r="G24" s="11">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H24" s="11">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I24" s="11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J24" s="11" t="s">
         <v>36</v>
       </c>
       <c r="K24" s="11"/>
-      <c r="L24" s="12"/>
+      <c r="L24" s="12" t="s">
+        <v>89</v>
+      </c>
       <c r="M24" s="12"/>
       <c r="N24" s="11"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="11"/>
       <c r="B25" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C25" s="11"/>
       <c r="D25" s="11" t="s">
@@ -1739,11 +1707,11 @@
       <c r="F25" s="11"/>
       <c r="G25" s="11">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H25" s="11">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I25" s="11">
         <v>2</v>
@@ -1759,7 +1727,7 @@
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="11"/>
       <c r="B26" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C26" s="11"/>
       <c r="D26" s="11" t="s">
@@ -1769,14 +1737,14 @@
       <c r="F26" s="11"/>
       <c r="G26" s="11">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H26" s="11">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I26" s="11">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="J26" s="11" t="s">
         <v>36</v>
@@ -1789,7 +1757,7 @@
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="11"/>
       <c r="B27" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C27" s="11"/>
       <c r="D27" s="11" t="s">
@@ -1799,14 +1767,14 @@
       <c r="F27" s="11"/>
       <c r="G27" s="11">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="H27" s="11">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I27" s="11">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J27" s="11" t="s">
         <v>36</v>
@@ -1819,7 +1787,7 @@
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="11"/>
       <c r="B28" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C28" s="11"/>
       <c r="D28" s="11" t="s">
@@ -1829,11 +1797,11 @@
       <c r="F28" s="11"/>
       <c r="G28" s="11">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H28" s="11">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="I28" s="11">
         <v>3</v>
@@ -1846,38 +1814,44 @@
       <c r="M28" s="12"/>
       <c r="N28" s="11"/>
     </row>
-    <row r="29" spans="1:14" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A29" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="B29" s="11"/>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" s="11"/>
+      <c r="B29" s="11" t="s">
+        <v>94</v>
+      </c>
       <c r="C29" s="11"/>
       <c r="D29" s="11" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="E29" s="11"/>
       <c r="F29" s="11"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="11"/>
-      <c r="I29" s="11"/>
+      <c r="G29" s="11">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="H29" s="11">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="I29" s="11">
+        <v>3</v>
+      </c>
       <c r="J29" s="11" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="K29" s="11"/>
       <c r="L29" s="12"/>
-      <c r="M29" s="12" t="s">
-        <v>96</v>
-      </c>
+      <c r="M29" s="12"/>
       <c r="N29" s="11"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B30" s="11"/>
       <c r="C30" s="11"/>
       <c r="D30" s="11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E30" s="11"/>
       <c r="F30" s="11"/>
@@ -1885,63 +1859,55 @@
       <c r="H30" s="11"/>
       <c r="I30" s="11"/>
       <c r="J30" s="11" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="K30" s="11"/>
       <c r="L30" s="12"/>
-      <c r="M30" s="12"/>
+      <c r="M30" s="12" t="s">
+        <v>96</v>
+      </c>
       <c r="N30" s="11"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A31" s="11"/>
-      <c r="B31" s="11" t="s">
-        <v>98</v>
-      </c>
+      <c r="A31" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="B31" s="11"/>
       <c r="C31" s="11"/>
       <c r="D31" s="11" t="s">
-        <v>61</v>
+        <v>34</v>
       </c>
       <c r="E31" s="11"/>
       <c r="F31" s="11"/>
-      <c r="G31" s="11">
-        <f t="shared" ref="G31:G48" si="2">+H30+1</f>
-        <v>1</v>
-      </c>
-      <c r="H31" s="11">
-        <f t="shared" ref="H31:H48" si="3">+H30+I31</f>
-        <v>3</v>
-      </c>
-      <c r="I31" s="11">
-        <v>3</v>
-      </c>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="11"/>
       <c r="J31" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K31" s="11"/>
-      <c r="L31" s="12" t="s">
-        <v>99</v>
-      </c>
+      <c r="L31" s="12"/>
       <c r="M31" s="12"/>
       <c r="N31" s="11"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="11"/>
       <c r="B32" s="11" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C32" s="11"/>
       <c r="D32" s="11" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="E32" s="11"/>
       <c r="F32" s="11"/>
       <c r="G32" s="11">
-        <f t="shared" si="2"/>
-        <v>4</v>
+        <f t="shared" ref="G32:G49" si="2">+H31+1</f>
+        <v>1</v>
       </c>
       <c r="H32" s="11">
-        <f t="shared" si="3"/>
-        <v>6</v>
+        <f t="shared" ref="H32:H49" si="3">+H31+I32</f>
+        <v>3</v>
       </c>
       <c r="I32" s="11">
         <v>3</v>
@@ -1950,31 +1916,35 @@
         <v>36</v>
       </c>
       <c r="K32" s="11"/>
-      <c r="L32" s="12"/>
+      <c r="L32" s="12" t="s">
+        <v>99</v>
+      </c>
       <c r="M32" s="12"/>
       <c r="N32" s="11"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="11"/>
       <c r="B33" s="11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C33" s="11"/>
       <c r="D33" s="11" t="s">
-        <v>37</v>
+        <v>124</v>
       </c>
       <c r="E33" s="11"/>
-      <c r="F33" s="11"/>
+      <c r="F33" s="11">
+        <v>999</v>
+      </c>
       <c r="G33" s="11">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H33" s="11">
         <f t="shared" si="3"/>
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="I33" s="11">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J33" s="11" t="s">
         <v>36</v>
@@ -1987,7 +1957,7 @@
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="11"/>
       <c r="B34" s="11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C34" s="11"/>
       <c r="D34" s="11" t="s">
@@ -1997,14 +1967,14 @@
       <c r="F34" s="11"/>
       <c r="G34" s="11">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="H34" s="11">
         <f t="shared" si="3"/>
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I34" s="11">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J34" s="11" t="s">
         <v>36</v>
@@ -2017,7 +1987,7 @@
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="11"/>
       <c r="B35" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C35" s="11"/>
       <c r="D35" s="11" t="s">
@@ -2027,14 +1997,14 @@
       <c r="F35" s="11"/>
       <c r="G35" s="11">
         <f t="shared" si="2"/>
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H35" s="11">
         <f t="shared" si="3"/>
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="I35" s="11">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="J35" s="11" t="s">
         <v>36</v>
@@ -2045,21 +2015,29 @@
       <c r="N35" s="11"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A36" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="B36" s="11"/>
+      <c r="A36" s="11"/>
+      <c r="B36" s="11" t="s">
+        <v>103</v>
+      </c>
       <c r="C36" s="11"/>
       <c r="D36" s="11" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E36" s="11"/>
       <c r="F36" s="11"/>
-      <c r="G36" s="11"/>
-      <c r="H36" s="11"/>
-      <c r="I36" s="11"/>
+      <c r="G36" s="11">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="H36" s="11">
+        <f t="shared" si="3"/>
+        <v>21</v>
+      </c>
+      <c r="I36" s="11">
+        <v>8</v>
+      </c>
       <c r="J36" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="K36" s="11"/>
       <c r="L36" s="12"/>
@@ -2067,71 +2045,63 @@
       <c r="N36" s="11"/>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A37" s="11"/>
-      <c r="B37" s="11" t="s">
-        <v>105</v>
-      </c>
+      <c r="A37" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="B37" s="11"/>
       <c r="C37" s="11"/>
       <c r="D37" s="11" t="s">
-        <v>61</v>
+        <v>34</v>
       </c>
       <c r="E37" s="11"/>
       <c r="F37" s="11"/>
-      <c r="G37" s="11">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="H37" s="11">
-        <f t="shared" si="3"/>
-        <v>3</v>
-      </c>
-      <c r="I37" s="11">
-        <v>3</v>
-      </c>
+      <c r="G37" s="11"/>
+      <c r="H37" s="11"/>
+      <c r="I37" s="11"/>
       <c r="J37" s="11" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="K37" s="11"/>
-      <c r="L37" s="12" t="s">
-        <v>106</v>
-      </c>
+      <c r="L37" s="12"/>
       <c r="M37" s="12"/>
       <c r="N37" s="11"/>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="11"/>
       <c r="B38" s="11" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C38" s="11"/>
       <c r="D38" s="11" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="E38" s="11"/>
       <c r="F38" s="11"/>
       <c r="G38" s="11">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H38" s="11">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I38" s="11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J38" s="11" t="s">
         <v>36</v>
       </c>
       <c r="K38" s="11"/>
-      <c r="L38" s="12"/>
+      <c r="L38" s="12" t="s">
+        <v>106</v>
+      </c>
       <c r="M38" s="12"/>
       <c r="N38" s="11"/>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="11"/>
       <c r="B39" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C39" s="11"/>
       <c r="D39" s="11" t="s">
@@ -2141,11 +2111,11 @@
       <c r="F39" s="11"/>
       <c r="G39" s="11">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H39" s="11">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I39" s="11">
         <v>2</v>
@@ -2161,7 +2131,7 @@
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="11"/>
       <c r="B40" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C40" s="11"/>
       <c r="D40" s="11" t="s">
@@ -2171,14 +2141,14 @@
       <c r="F40" s="11"/>
       <c r="G40" s="11">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H40" s="11">
         <f t="shared" si="3"/>
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="I40" s="11">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J40" s="11" t="s">
         <v>36</v>
@@ -2191,7 +2161,7 @@
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="11"/>
       <c r="B41" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C41" s="11"/>
       <c r="D41" s="11" t="s">
@@ -2201,14 +2171,14 @@
       <c r="F41" s="11"/>
       <c r="G41" s="11">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="H41" s="11">
         <f t="shared" si="3"/>
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="I41" s="11">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J41" s="11" t="s">
         <v>36</v>
@@ -2218,128 +2188,136 @@
       <c r="M41" s="12"/>
       <c r="N41" s="11"/>
     </row>
-    <row r="42" spans="1:14" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A42" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="B42" s="11"/>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A42" s="11"/>
+      <c r="B42" s="11" t="s">
+        <v>110</v>
+      </c>
       <c r="C42" s="11"/>
       <c r="D42" s="11" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E42" s="11"/>
       <c r="F42" s="11"/>
-      <c r="G42" s="11"/>
-      <c r="H42" s="11"/>
-      <c r="I42" s="11"/>
-      <c r="J42" s="11"/>
+      <c r="G42" s="11">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="H42" s="11">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="I42" s="11">
+        <v>5</v>
+      </c>
+      <c r="J42" s="11" t="s">
+        <v>36</v>
+      </c>
       <c r="K42" s="11"/>
       <c r="L42" s="12"/>
-      <c r="M42" s="12" t="s">
-        <v>112</v>
-      </c>
+      <c r="M42" s="12"/>
       <c r="N42" s="11"/>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B43" s="11"/>
       <c r="C43" s="11"/>
       <c r="D43" s="11" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="E43" s="11"/>
       <c r="F43" s="11"/>
       <c r="G43" s="11"/>
       <c r="H43" s="11"/>
       <c r="I43" s="11"/>
-      <c r="J43" s="11" t="s">
-        <v>35</v>
-      </c>
+      <c r="J43" s="11"/>
       <c r="K43" s="11"/>
       <c r="L43" s="12"/>
-      <c r="M43" s="12"/>
+      <c r="M43" s="12" t="s">
+        <v>112</v>
+      </c>
       <c r="N43" s="11"/>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A44" s="11"/>
-      <c r="B44" s="11" t="s">
-        <v>114</v>
-      </c>
+      <c r="A44" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="B44" s="11"/>
       <c r="C44" s="11"/>
       <c r="D44" s="11" t="s">
-        <v>61</v>
+        <v>34</v>
       </c>
       <c r="E44" s="11"/>
       <c r="F44" s="11"/>
-      <c r="G44" s="11">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="H44" s="11">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="I44" s="11">
-        <v>2</v>
-      </c>
+      <c r="G44" s="11"/>
+      <c r="H44" s="11"/>
+      <c r="I44" s="11"/>
       <c r="J44" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K44" s="11"/>
-      <c r="L44" s="12" t="s">
-        <v>115</v>
-      </c>
+      <c r="L44" s="12"/>
       <c r="M44" s="12"/>
       <c r="N44" s="11"/>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="11"/>
       <c r="B45" s="11" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C45" s="11"/>
       <c r="D45" s="11" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="E45" s="11"/>
       <c r="F45" s="11"/>
       <c r="G45" s="11">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H45" s="11">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="I45" s="11">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J45" s="11" t="s">
         <v>36</v>
       </c>
       <c r="K45" s="11"/>
-      <c r="L45" s="12"/>
+      <c r="L45" s="12" t="s">
+        <v>115</v>
+      </c>
       <c r="M45" s="12"/>
       <c r="N45" s="11"/>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A46" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="B46" s="11"/>
+      <c r="A46" s="11"/>
+      <c r="B46" s="11" t="s">
+        <v>116</v>
+      </c>
       <c r="C46" s="11"/>
       <c r="D46" s="11" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E46" s="11"/>
       <c r="F46" s="11"/>
-      <c r="G46" s="11"/>
-      <c r="H46" s="11"/>
-      <c r="I46" s="11"/>
+      <c r="G46" s="11">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="H46" s="11">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="I46" s="11">
+        <v>5</v>
+      </c>
       <c r="J46" s="11" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="K46" s="11"/>
       <c r="L46" s="12"/>
@@ -2347,88 +2325,110 @@
       <c r="N46" s="11"/>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A47" s="11"/>
-      <c r="B47" s="11" t="s">
-        <v>118</v>
-      </c>
+      <c r="A47" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="B47" s="11"/>
       <c r="C47" s="11"/>
       <c r="D47" s="11" t="s">
-        <v>61</v>
+        <v>34</v>
       </c>
       <c r="E47" s="11"/>
       <c r="F47" s="11"/>
-      <c r="G47" s="11">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="H47" s="11">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="I47" s="11">
-        <v>2</v>
-      </c>
+      <c r="G47" s="11"/>
+      <c r="H47" s="11"/>
+      <c r="I47" s="11"/>
       <c r="J47" s="11" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="K47" s="11"/>
-      <c r="L47" s="12" t="s">
-        <v>119</v>
-      </c>
+      <c r="L47" s="12"/>
       <c r="M47" s="12"/>
       <c r="N47" s="11"/>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="11"/>
       <c r="B48" s="11" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C48" s="11"/>
       <c r="D48" s="11" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="E48" s="11"/>
       <c r="F48" s="11"/>
       <c r="G48" s="11">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H48" s="11">
         <f t="shared" si="3"/>
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="I48" s="11">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="J48" s="11" t="s">
         <v>36</v>
       </c>
       <c r="K48" s="11"/>
-      <c r="L48" s="12"/>
+      <c r="L48" s="12" t="s">
+        <v>119</v>
+      </c>
       <c r="M48" s="12"/>
       <c r="N48" s="11"/>
     </row>
-    <row r="49" spans="1:14" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A49" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="B49" s="11"/>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A49" s="11"/>
+      <c r="B49" s="11" t="s">
+        <v>120</v>
+      </c>
       <c r="C49" s="11"/>
       <c r="D49" s="11" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E49" s="11"/>
       <c r="F49" s="11"/>
-      <c r="G49" s="11"/>
-      <c r="H49" s="11"/>
-      <c r="I49" s="11"/>
-      <c r="J49" s="11"/>
+      <c r="G49" s="11">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="H49" s="11">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="I49" s="11">
+        <v>10</v>
+      </c>
+      <c r="J49" s="11" t="s">
+        <v>36</v>
+      </c>
       <c r="K49" s="11"/>
       <c r="L49" s="12"/>
-      <c r="M49" s="12" t="s">
+      <c r="M49" s="12"/>
+      <c r="N49" s="11"/>
+    </row>
+    <row r="50" spans="1:14" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A50" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B50" s="11"/>
+      <c r="C50" s="11"/>
+      <c r="D50" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E50" s="11"/>
+      <c r="F50" s="11"/>
+      <c r="G50" s="11"/>
+      <c r="H50" s="11"/>
+      <c r="I50" s="11"/>
+      <c r="J50" s="11"/>
+      <c r="K50" s="11"/>
+      <c r="L50" s="12"/>
+      <c r="M50" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="N49" s="11"/>
+      <c r="N50" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>